<commit_message>
Comecei a estruturar o projeto por pastas.
</commit_message>
<xml_diff>
--- a/Presenca.xlsx
+++ b/Presenca.xlsx
@@ -6,9 +6,10 @@
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9600" windowWidth="21600" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="09_01" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="08_01" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="06_01" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="10_01" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="09_01" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="08_01" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="06_01" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -348,8 +349,8 @@
   </sheetPr>
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="A4:E7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -362,7 +363,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>09/01/20</t>
+          <t>10/01/20</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -389,7 +390,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>15:36</t>
+          <t>18:34</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -411,7 +412,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>15:45</t>
+          <t>18:36</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -431,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E7" sqref="A4:E7"/>
@@ -447,7 +448,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>08/01/20</t>
+          <t>09/01/20</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
@@ -458,6 +459,50 @@
       <c r="D1" t="inlineStr">
         <is>
           <t>Empresa</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Gabriel Taranto</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>15:36</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>ICA</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Gabriel Taranto</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Presente</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>15:45</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>ICA</t>
         </is>
       </c>
     </row>
@@ -488,6 +533,47 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>08/01/20</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Hora</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Empresa</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="A4:E7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Nome</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>06/01/20</t>
         </is>
       </c>

</xml_diff>